<commit_message>
adição de todas as partes
adição de partes e readicionar o 1 excel da segunda experiencia
</commit_message>
<xml_diff>
--- a/MCE_PL5_G5_T21.xlsx
+++ b/MCE_PL5_G5_T21.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Documents\GitHub\MCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\repol\Dropbox\MCE\PL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C59E5F6-EBAF-4611-829D-74FB2E23BC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54F87F9-8A21-4D0F-AD65-C404CEC2C277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1323,707 +1322,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Tensão de Hall em função da Intensidade</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.28385116992711928"/>
-          <c:y val="1.3488450514247175E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="8.1067930375216327E-2"/>
-          <c:y val="8.075572495774902E-2"/>
-          <c:w val="0.89179299221659436"/>
-          <c:h val="0.76403150668381925"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Folha1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Folha1!$C$2:$C$30</c:f>
-              <c:strCache>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>I(A)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0,03</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0,05</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0,07</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0,09</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0,11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0,13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0,15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0,17</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0,19</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0,21</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0,23</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0,25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0,27</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0,29</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0,31</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0,33</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0,35</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0,37</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0,39</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0,41</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0,43</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0,45</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0,47</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0,49</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0,51</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0,53</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0,55</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Folha1!$B$2:$B$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.8000000000000014E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1599999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4199999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7299999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.01E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3199999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.5700000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.8799999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.1300000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.3799999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.6999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.9600000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.1799999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.4899999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.8500000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.0500000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.33E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.62E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.9299999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6.1799999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6.4500000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.6700000000000009E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7.3799999999999991E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7.5499999999999998E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-392C-4445-9A0C-95849421BE66}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="662320848"/>
-        <c:axId val="662320208"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="662320848"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-PT"/>
-                  <a:t>Intensidade</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="pt-PT" baseline="0"/>
-                  <a:t> (A)</a:t>
-                </a:r>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="662320208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="662320208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pt-PT"/>
-                  <a:t>Tensão</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="pt-PT" baseline="0"/>
-                  <a:t> de Hall (V)</a:t>
-                </a:r>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="6.7311206352370515E-3"/>
-              <c:y val="0.3285106812331311"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="662320848"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2104,46 +1402,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3172,555 +2430,6 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3794,45 +2503,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>70485</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FEA476F-CAC0-4C15-82AB-59FB70634E16}"/>
-            </a:ext>
-            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4140,8 +2810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>